<commit_message>
Trying outlier detection adding ao only
</commit_message>
<xml_diff>
--- a/fcst_results/arima_with_outliers_summary_stats_HOU-Dom.xlsx
+++ b/fcst_results/arima_with_outliers_summary_stats_HOU-Dom.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,401 +468,201 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>LS2001Sep</t>
+          <t>AO2008Sep</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-170700</v>
+        <v>-134900</v>
       </c>
       <c r="C2" t="n">
-        <v>56200</v>
+        <v>38900</v>
       </c>
       <c r="D2" t="n">
-        <v>-3.038</v>
+        <v>-3.471</v>
       </c>
       <c r="E2" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F2" t="n">
-        <v>-281000</v>
+        <v>-211000</v>
       </c>
       <c r="G2" t="n">
-        <v>-60600</v>
+        <v>-58700</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>AO2008Sep</t>
+          <t>AO2020Mar</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-134900</v>
+        <v>22960</v>
       </c>
       <c r="C3" t="n">
-        <v>36700</v>
+        <v>10500</v>
       </c>
       <c r="D3" t="n">
-        <v>-3.673</v>
+        <v>2.192</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.028</v>
       </c>
       <c r="F3" t="n">
-        <v>-207000</v>
+        <v>2429.908</v>
       </c>
       <c r="G3" t="n">
-        <v>-62900</v>
+        <v>43500</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>LS2017Aug</t>
+          <t>ar.L1</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-142400</v>
+        <v>0.8799</v>
       </c>
       <c r="C4" t="n">
-        <v>34500</v>
+        <v>0.055</v>
       </c>
       <c r="D4" t="n">
-        <v>-4.123</v>
+        <v>15.995</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>-210000</v>
+        <v>0.772</v>
       </c>
       <c r="G4" t="n">
-        <v>-74700</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>LS2017Oct</t>
+          <t>ma.L1</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>153900</v>
+        <v>-0.8314</v>
       </c>
       <c r="C5" t="n">
-        <v>42800</v>
+        <v>0.079</v>
       </c>
       <c r="D5" t="n">
-        <v>3.596</v>
+        <v>-10.475</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>70000</v>
+        <v>-0.987</v>
       </c>
       <c r="G5" t="n">
-        <v>238000</v>
+        <v>-0.676</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>AO2020Mar</t>
+          <t>ma.L2</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>249200</v>
+        <v>-0.1528</v>
       </c>
       <c r="C6" t="n">
-        <v>11100</v>
+        <v>0.063</v>
       </c>
       <c r="D6" t="n">
-        <v>22.467</v>
+        <v>-2.43</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.015</v>
       </c>
       <c r="F6" t="n">
-        <v>227000</v>
+        <v>-0.276</v>
       </c>
       <c r="G6" t="n">
-        <v>271000</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>LS2020Mar</t>
+          <t>ar.S.L12</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-452400</v>
+        <v>0.9617</v>
       </c>
       <c r="C7" t="n">
-        <v>11100</v>
+        <v>0.027</v>
       </c>
       <c r="D7" t="n">
-        <v>-40.785</v>
+        <v>36.099</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>-474000</v>
+        <v>0.909</v>
       </c>
       <c r="G7" t="n">
-        <v>-431000</v>
+        <v>1.014</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>LS2020Jun</t>
+          <t>ma.S.L12</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>122900</v>
+        <v>-0.8188</v>
       </c>
       <c r="C8" t="n">
-        <v>63400</v>
+        <v>0.064</v>
       </c>
       <c r="D8" t="n">
-        <v>1.938</v>
+        <v>-12.871</v>
       </c>
       <c r="E8" t="n">
-        <v>0.053</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>-1405.989</v>
+        <v>-0.9429999999999999</v>
       </c>
       <c r="G8" t="n">
-        <v>247000</v>
+        <v>-0.694</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>LS2020Aug</t>
+          <t>sigma2</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>16850</v>
+        <v>2361000000</v>
       </c>
       <c r="C9" t="n">
-        <v>41000</v>
+        <v>0.731</v>
       </c>
       <c r="D9" t="n">
-        <v>0.411</v>
+        <v>3230000000</v>
       </c>
       <c r="E9" t="n">
-        <v>0.681</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>-63400</v>
+        <v>2360000000</v>
       </c>
       <c r="G9" t="n">
-        <v>97100</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>LS2020Dec</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>62190</v>
-      </c>
-      <c r="C10" t="n">
-        <v>188000</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.331</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="F10" t="n">
-        <v>-306000</v>
-      </c>
-      <c r="G10" t="n">
-        <v>430000</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>LS2021Mar</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>193200</v>
-      </c>
-      <c r="C11" t="n">
-        <v>30800</v>
-      </c>
-      <c r="D11" t="n">
-        <v>6.277</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>133000</v>
-      </c>
-      <c r="G11" t="n">
-        <v>253000</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>ar.L1</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0.4155</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.781</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.532</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.595</v>
-      </c>
-      <c r="F12" t="n">
-        <v>-1.115</v>
-      </c>
-      <c r="G12" t="n">
-        <v>1.946</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>ma.L1</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>-0.586</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.805</v>
-      </c>
-      <c r="D13" t="n">
-        <v>-0.728</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.467</v>
-      </c>
-      <c r="F13" t="n">
-        <v>-2.165</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.993</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>ma.L2</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>0.0097</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.171</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.057</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.955</v>
-      </c>
-      <c r="F14" t="n">
-        <v>-0.325</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.344</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>ar.S.L12</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>0.9262</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.044</v>
-      </c>
-      <c r="D15" t="n">
-        <v>21.12</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="G15" t="n">
-        <v>1.012</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>ma.S.L12</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>-0.7254</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.08799999999999999</v>
-      </c>
-      <c r="D16" t="n">
-        <v>-8.244</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" t="n">
-        <v>-0.898</v>
-      </c>
-      <c r="G16" t="n">
-        <v>-0.553</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>sigma2</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>1417000000</v>
-      </c>
-      <c r="C17" t="n">
-        <v>13.654</v>
-      </c>
-      <c r="D17" t="n">
-        <v>104000000</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="n">
-        <v>1420000000</v>
-      </c>
-      <c r="G17" t="n">
-        <v>1420000000</v>
+        <v>2360000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>